<commit_message>
Conf file management updated to avoid overwritting, SVM finished
</commit_message>
<xml_diff>
--- a/Configurations/ConfigurationResults.xlsx
+++ b/Configurations/ConfigurationResults.xlsx
@@ -7,28 +7,28 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Complete" sheetId="1" r:id="rId1"/>
+    <sheet name="CompleteSVM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
   <si>
     <t>Conf_id</t>
   </si>
   <si>
-    <t>Criterion</t>
-  </si>
-  <si>
-    <t>max_depth</t>
-  </si>
-  <si>
-    <t>n_estimators</t>
-  </si>
-  <si>
-    <t>max_features</t>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Gamma</t>
   </si>
   <si>
     <t>P1</t>
@@ -49,10 +49,16 @@
     <t>Promedio</t>
   </si>
   <si>
-    <t>gini</t>
-  </si>
-  <si>
-    <t>entropy</t>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -461,32 +467,32 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>5</v>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
       <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
+        <v>0.001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
       </c>
       <c r="G2">
-        <v>0.8325795005153743</v>
+        <v>0.1915484268969772</v>
       </c>
       <c r="H2">
-        <v>0.8645444518226575</v>
+        <v>0.1865203761755486</v>
       </c>
       <c r="I2">
-        <v>0.8531229754300952</v>
+        <v>0.1839443742098609</v>
       </c>
       <c r="J2">
-        <v>0.8608294132638069</v>
+        <v>0.1837444655281467</v>
       </c>
       <c r="K2">
-        <v>0.8287632096495157</v>
+        <v>0.1898263027295285</v>
       </c>
       <c r="L2">
-        <v>0.8479679101362899</v>
+        <v>0.1871167891080124</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -499,32 +505,32 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>7</v>
+      <c r="D3" t="s">
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
+        <v>0.01</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
       </c>
       <c r="G3">
-        <v>0.946959606640858</v>
+        <v>0.6808098560552988</v>
       </c>
       <c r="H3">
-        <v>0.9687825838788646</v>
+        <v>0.6767517672393788</v>
       </c>
       <c r="I3">
-        <v>0.9644215744537188</v>
+        <v>0.6793398127806943</v>
       </c>
       <c r="J3">
-        <v>0.9648336932905753</v>
+        <v>0.666273698520587</v>
       </c>
       <c r="K3">
-        <v>0.9728458049886621</v>
+        <v>0.670045632106979</v>
       </c>
       <c r="L3">
-        <v>0.9635686526505358</v>
+        <v>0.6746441533405877</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -537,32 +543,32 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>10</v>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>9</v>
+        <v>0.05</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>0.9834737848387713</v>
+        <v>0.9538322171813265</v>
       </c>
       <c r="H4">
-        <v>0.9861300819930156</v>
+        <v>0.9489665752304639</v>
       </c>
       <c r="I4">
-        <v>0.9845576833175604</v>
+        <v>0.9581775081535457</v>
       </c>
       <c r="J4">
-        <v>0.9870132427856836</v>
+        <v>0.9601877803619121</v>
       </c>
       <c r="K4">
-        <v>0.9865296297233899</v>
+        <v>0.9643856934411672</v>
       </c>
       <c r="L4">
-        <v>0.9855408845316841</v>
+        <v>0.9571099548736832</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -575,32 +581,32 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
-        <v>150</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
       <c r="G5">
-        <v>0.9866197297535931</v>
+        <v>0.9718942018997925</v>
       </c>
       <c r="H5">
-        <v>0.9827953173719649</v>
+        <v>0.9638326935920185</v>
       </c>
       <c r="I5">
-        <v>0.9883974399899892</v>
+        <v>0.9718936794945821</v>
       </c>
       <c r="J5">
-        <v>0.9876448035529186</v>
+        <v>0.9749476844002911</v>
       </c>
       <c r="K5">
-        <v>0.9879764918272365</v>
+        <v>0.9754344732906393</v>
       </c>
       <c r="L5">
-        <v>0.9866867564991404</v>
+        <v>0.9716005465354648</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -613,32 +619,32 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6">
-        <v>15</v>
+      <c r="D6" t="s">
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>200</v>
-      </c>
-      <c r="F6">
-        <v>21</v>
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
       </c>
       <c r="G6">
-        <v>0.9844684632172798</v>
+        <v>0.9867942008844881</v>
       </c>
       <c r="H6">
-        <v>0.9827123297731316</v>
+        <v>0.9839995261344443</v>
       </c>
       <c r="I6">
-        <v>0.9889422779999597</v>
+        <v>0.9883033215669523</v>
       </c>
       <c r="J6">
-        <v>0.9862404374789</v>
+        <v>0.9886695954093215</v>
       </c>
       <c r="K6">
-        <v>0.9887237649562836</v>
+        <v>0.9878862125037932</v>
       </c>
       <c r="L6">
-        <v>0.986217454685111</v>
+        <v>0.9871305712997998</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -651,32 +657,32 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
-        <v>17</v>
+      <c r="D7" t="s">
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>400</v>
-      </c>
-      <c r="F7">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>0.9859818256359997</v>
+        <v>0.9902654105274939</v>
       </c>
       <c r="H7">
-        <v>0.9854770273319811</v>
+        <v>0.9874977058375438</v>
       </c>
       <c r="I7">
-        <v>0.9893589473324784</v>
+        <v>0.9891673775946608</v>
       </c>
       <c r="J7">
-        <v>0.9862482910246462</v>
+        <v>0.9911226669678685</v>
       </c>
       <c r="K7">
-        <v>0.9879511207873048</v>
+        <v>0.9888643044701797</v>
       </c>
       <c r="L7">
-        <v>0.9870034424224819</v>
+        <v>0.9893834930795492</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -689,32 +695,32 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8">
-        <v>21</v>
+      <c r="D8" t="s">
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>500</v>
-      </c>
-      <c r="F8">
-        <v>18</v>
+        <v>1.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>0.9859818256359997</v>
+        <v>0.9902157034865668</v>
       </c>
       <c r="H8">
-        <v>0.9843124678604996</v>
+        <v>0.9880919409788653</v>
       </c>
       <c r="I8">
-        <v>0.9900896201119369</v>
+        <v>0.9884427426472988</v>
       </c>
       <c r="J8">
-        <v>0.9866551214847697</v>
+        <v>0.9909375427808046</v>
       </c>
       <c r="K8">
-        <v>0.9891552762533938</v>
+        <v>0.99123273568448</v>
       </c>
       <c r="L8">
-        <v>0.9872388622693199</v>
+        <v>0.989784133115603</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -727,32 +733,32 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9">
-        <v>10</v>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>150</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
       </c>
       <c r="G9">
-        <v>0.9823549115601135</v>
+        <v>0.9919474211050463</v>
       </c>
       <c r="H9">
-        <v>0.9823540299664913</v>
+        <v>0.9889594355443792</v>
       </c>
       <c r="I9">
-        <v>0.9835884712709482</v>
+        <v>0.9892269793895476</v>
       </c>
       <c r="J9">
-        <v>0.9855663549890761</v>
+        <v>0.9897325931167074</v>
       </c>
       <c r="K9">
-        <v>0.9886887859009407</v>
+        <v>0.992212723776809</v>
       </c>
       <c r="L9">
-        <v>0.9845105107375138</v>
+        <v>0.9904158305864978</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -763,34 +769,34 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>13</v>
+        <v>0.001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
       </c>
       <c r="G10">
-        <v>0.842998014802501</v>
+        <v>0.1915484268969772</v>
       </c>
       <c r="H10">
-        <v>0.8731302313542694</v>
+        <v>0.1865203761755486</v>
       </c>
       <c r="I10">
-        <v>0.867838460583813</v>
+        <v>0.1839443742098609</v>
       </c>
       <c r="J10">
-        <v>0.8480031045040193</v>
+        <v>0.1837444655281467</v>
       </c>
       <c r="K10">
-        <v>0.8794549471926587</v>
+        <v>0.1898263027295285</v>
       </c>
       <c r="L10">
-        <v>0.8622849516874522</v>
+        <v>0.1871167891080124</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -801,34 +807,34 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>30</v>
-      </c>
-      <c r="F11">
-        <v>15</v>
+        <v>0.01</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
       </c>
       <c r="G11">
-        <v>0.9570388605666443</v>
+        <v>0.6808098560552988</v>
       </c>
       <c r="H11">
-        <v>0.9535972795348739</v>
+        <v>0.6767517672393788</v>
       </c>
       <c r="I11">
-        <v>0.9679210436599776</v>
+        <v>0.6793398127806943</v>
       </c>
       <c r="J11">
-        <v>0.9644752299821845</v>
+        <v>0.666273698520587</v>
       </c>
       <c r="K11">
-        <v>0.9529181858072143</v>
+        <v>0.670045632106979</v>
       </c>
       <c r="L11">
-        <v>0.9591901199101789</v>
+        <v>0.6746441533405877</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -839,34 +845,34 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
       </c>
       <c r="E12">
-        <v>100</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
+        <v>0.05</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
       </c>
       <c r="G12">
-        <v>0.9854922720789322</v>
+        <v>0.9538322171813265</v>
       </c>
       <c r="H12">
-        <v>0.9842621220927925</v>
+        <v>0.9489665752304639</v>
       </c>
       <c r="I12">
-        <v>0.9843141474280288</v>
+        <v>0.9581775081535457</v>
       </c>
       <c r="J12">
-        <v>0.9857377754937948</v>
+        <v>0.9601877803619121</v>
       </c>
       <c r="K12">
-        <v>0.9902011866280012</v>
+        <v>0.9643856934411672</v>
       </c>
       <c r="L12">
-        <v>0.9860015007443099</v>
+        <v>0.9571099548736832</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -877,34 +883,34 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
       </c>
       <c r="E13">
-        <v>150</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
       </c>
       <c r="G13">
-        <v>0.9831765552257736</v>
+        <v>0.9718942018997925</v>
       </c>
       <c r="H13">
-        <v>0.9848463451693061</v>
+        <v>0.9638326935920185</v>
       </c>
       <c r="I13">
-        <v>0.9809258904894056</v>
+        <v>0.9718936794945821</v>
       </c>
       <c r="J13">
-        <v>0.9854082633899857</v>
+        <v>0.9749476844002911</v>
       </c>
       <c r="K13">
-        <v>0.9892216726283445</v>
+        <v>0.9754344732906393</v>
       </c>
       <c r="L13">
-        <v>0.9847157453805633</v>
+        <v>0.9716005465354648</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -915,34 +921,34 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
       </c>
       <c r="E14">
-        <v>200</v>
-      </c>
-      <c r="F14">
-        <v>21</v>
+        <v>0.5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
       </c>
       <c r="G14">
-        <v>0.9847957327907242</v>
+        <v>0.9867942008844881</v>
       </c>
       <c r="H14">
-        <v>0.9812305355349445</v>
+        <v>0.9839995261344443</v>
       </c>
       <c r="I14">
-        <v>0.9883204095698519</v>
+        <v>0.9883033215669523</v>
       </c>
       <c r="J14">
-        <v>0.9891019501417627</v>
+        <v>0.9886695954093215</v>
       </c>
       <c r="K14">
-        <v>0.9897101335033677</v>
+        <v>0.9878862125037932</v>
       </c>
       <c r="L14">
-        <v>0.9866317523081302</v>
+        <v>0.9871305712997998</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -953,34 +959,34 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
       </c>
       <c r="E15">
-        <v>400</v>
-      </c>
-      <c r="F15">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
       </c>
       <c r="G15">
-        <v>0.9854391182344027</v>
+        <v>0.9902654105274939</v>
       </c>
       <c r="H15">
-        <v>0.9830002504463446</v>
+        <v>0.9874977058375438</v>
       </c>
       <c r="I15">
-        <v>0.987559543414679</v>
+        <v>0.9891673775946608</v>
       </c>
       <c r="J15">
-        <v>0.9891124113110461</v>
+        <v>0.9911226669678685</v>
       </c>
       <c r="K15">
-        <v>0.9922671004419914</v>
+        <v>0.9888643044701797</v>
       </c>
       <c r="L15">
-        <v>0.9874756847696927</v>
+        <v>0.9893834930795492</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -991,34 +997,34 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>500</v>
-      </c>
-      <c r="F16">
-        <v>15</v>
+        <v>1.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
       </c>
       <c r="G16">
-        <v>0.9858756753497353</v>
+        <v>0.9902157034865668</v>
       </c>
       <c r="H16">
-        <v>0.9839232517974424</v>
+        <v>0.9880919409788653</v>
       </c>
       <c r="I16">
-        <v>0.9865770710328546</v>
+        <v>0.9884427426472988</v>
       </c>
       <c r="J16">
-        <v>0.9874770812355094</v>
+        <v>0.9909375427808046</v>
       </c>
       <c r="K16">
-        <v>0.9905544726521218</v>
+        <v>0.99123273568448</v>
       </c>
       <c r="L16">
-        <v>0.9868815104135326</v>
+        <v>0.989784133115603</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1029,34 +1035,34 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
       </c>
       <c r="E17">
-        <v>150</v>
-      </c>
-      <c r="F17">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
       </c>
       <c r="G17">
-        <v>0.9823549115601135</v>
+        <v>0.9919474211050463</v>
       </c>
       <c r="H17">
-        <v>0.9797564339979072</v>
+        <v>0.9889594355443792</v>
       </c>
       <c r="I17">
-        <v>0.9835884712709482</v>
+        <v>0.9892269793895476</v>
       </c>
       <c r="J17">
-        <v>0.9857954004657489</v>
+        <v>0.9897325931167074</v>
       </c>
       <c r="K17">
-        <v>0.9882916425812327</v>
+        <v>0.992212723776809</v>
       </c>
       <c r="L17">
-        <v>0.9839573719751901</v>
+        <v>0.9904158305864978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Configurations file renamed from HyperparametersRF to Hyperparameters
</commit_message>
<xml_diff>
--- a/Configurations/ConfigurationResults.xlsx
+++ b/Configurations/ConfigurationResults.xlsx
@@ -11,6 +11,7 @@
     <sheet name="CompleteRFC" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="CompleteNB" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="CompleteNB1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CompleteRFC1" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -3107,4 +3108,805 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Criterion</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>max_depth</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>n_estimators</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>max_features</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8082813012803404</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8047662376139391</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.7861722212162833</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.7742819099071137</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.8177520061402811</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.7982507352315914</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9614932441097477</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9522535577528214</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9496338346378987</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9290591409681976</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9398414431196858</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.9464562441176703</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.985740541262185</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9827410729132375</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.985667235573898</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9855146623457041</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.9855509657450032</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.9850428955680055</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F5" t="n">
+        <v>150</v>
+      </c>
+      <c r="G5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9852105060606411</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9841173026983225</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.989763917212975</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9890683669299062</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9906418203275371</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9877603826458763</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" t="n">
+        <v>21</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9871561711599128</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.9848347327925404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.9905007847468091</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9863879619576181</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9917160574374575</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.9881191416188676</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="n">
+        <v>400</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9854234449234226</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9861011768307386</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.9889985263520042</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.9864200181289061</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.9907442279034873</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9875374788277117</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>21</v>
+      </c>
+      <c r="F8" t="n">
+        <v>500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>18</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9846924928332484</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.985146133179174</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.9889985263520042</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9878342470258968</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.9917160574374575</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.9876774913655563</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>150</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9847755178524658</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9814632114151935</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.9827844301601295</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.9867877909273719</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.9862817597689497</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.9844185420248222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>13</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.8268748805871683</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.8086577251796926</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.842807864571653</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.8154401136565022</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.8428246127280945</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.8273210393446222</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9624350795053922</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.9455367976390423</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9682938902993993</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.9624472419109688</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.9650367735341482</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.9607499565777902</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9862806813923686</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.9820324469646149</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.9802179160167925</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9849648832414222</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.9905162072216733</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.9848024269673742</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
+      <c r="F13" t="n">
+        <v>150</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9777663503945369</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.9795182192488896</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.9723756786386794</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.9843260474196867</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.9826680716890173</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.9793308734781618</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>15</v>
+      </c>
+      <c r="F14" t="n">
+        <v>200</v>
+      </c>
+      <c r="G14" t="n">
+        <v>21</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9850344774743822</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.9793058050422392</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.9891717250110007</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.9849878298975374</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.9913037542948692</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.9859607183440058</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>17</v>
+      </c>
+      <c r="F15" t="n">
+        <v>400</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9858502955861703</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.9842008947337588</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.9891511721149359</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.9882685347127076</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.9918370519325963</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.9878615898160337</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9859419079025691</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.9836645759570886</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.9889375881764481</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.9868532508086646</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.993247526687467</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.9877289699064475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>150</v>
+      </c>
+      <c r="G17" t="n">
+        <v>12</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9852143264489701</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.9819171589060189</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.9833446074080839</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9871951616772192</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.9870642026677869</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.9849470914216157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RFC model trained and saved
</commit_message>
<xml_diff>
--- a/Configurations/ConfigurationResults.xlsx
+++ b/Configurations/ConfigurationResults.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10420" windowWidth="19420" xWindow="-110" yWindow="-110"/>
+    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="5" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7365" windowWidth="14400" xWindow="38595" yWindow="2775"/>
   </bookViews>
   <sheets>
     <sheet name="CompleteSVM" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,6 +12,9 @@
     <sheet name="CompleteNB" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="CompleteNB1" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="CompleteRFC1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CompleteRFC2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="CompleteRFC3" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="CompleteRFC4" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,6 +46,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -54,12 +62,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -103,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -112,6 +135,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2842,7 +2868,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -2948,7 +2974,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="3" t="inlineStr">
@@ -3118,6 +3144,1608 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Criterion</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>max_depth</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>n_estimators</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>max_features</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8082813012803404</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8047662376139391</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.7861722212162833</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.7742819099071137</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.8177520061402811</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.7982507352315914</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9614932441097477</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9522535577528214</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9496338346378987</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9290591409681976</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9398414431196858</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.9464562441176703</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.985740541262185</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9827410729132375</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.985667235573898</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9855146623457041</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.9855509657450032</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.9850428955680055</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F5" t="n">
+        <v>150</v>
+      </c>
+      <c r="G5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9852105060606411</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9841173026983225</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.989763917212975</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9890683669299062</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9906418203275371</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9877603826458763</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" t="n">
+        <v>21</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9871561711599128</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.9848347327925404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.9905007847468091</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9863879619576181</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9917160574374575</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.9881191416188676</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="n">
+        <v>400</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9854234449234226</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9861011768307386</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.9889985263520042</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.9864200181289061</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.9907442279034873</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9875374788277117</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>21</v>
+      </c>
+      <c r="F8" t="n">
+        <v>500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>18</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9846924928332484</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.985146133179174</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.9889985263520042</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9878342470258968</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.9917160574374575</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.9876774913655563</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>150</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9847755178524658</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9814632114151935</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.9827844301601295</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.9867877909273719</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.9862817597689497</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.9844185420248222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>13</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.8268748805871683</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.8086577251796926</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.842807864571653</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.8154401136565022</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.8428246127280945</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.8273210393446222</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9624350795053922</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.9455367976390423</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9682938902993993</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.9624472419109688</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.9650367735341482</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.9607499565777902</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9862806813923686</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.9820324469646149</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.9802179160167925</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9849648832414222</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.9905162072216733</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.9848024269673742</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
+      <c r="F13" t="n">
+        <v>150</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9777663503945369</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.9795182192488896</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.9723756786386794</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.9843260474196867</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.9826680716890173</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.9793308734781618</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>15</v>
+      </c>
+      <c r="F14" t="n">
+        <v>200</v>
+      </c>
+      <c r="G14" t="n">
+        <v>21</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9850344774743822</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.9793058050422392</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.9891717250110007</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.9849878298975374</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.9913037542948692</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.9859607183440058</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>17</v>
+      </c>
+      <c r="F15" t="n">
+        <v>400</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9858502955861703</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.9842008947337588</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.9891511721149359</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.9882685347127076</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.9918370519325963</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.9878615898160337</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9859419079025691</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.9836645759570886</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.9889375881764481</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.9868532508086646</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.993247526687467</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.9877289699064475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>150</v>
+      </c>
+      <c r="G17" t="n">
+        <v>12</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9852143264489701</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.9819171589060189</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.9833446074080839</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9871951616772192</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.9870642026677869</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.9849470914216157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Criterion</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>max_depth</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>n_estimators</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>max_features</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8082813012803404</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8047662376139391</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.7861722212162833</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.7742819099071137</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.8177520061402811</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.7982507352315914</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9614932441097477</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9522535577528214</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9496338346378987</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9290591409681976</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9398414431196858</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.9464562441176703</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.985740541262185</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9827410729132375</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.985667235573898</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9855146623457041</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.9855509657450032</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.9850428955680055</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F5" t="n">
+        <v>150</v>
+      </c>
+      <c r="G5" t="n">
+        <v>15</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9852105060606411</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9841173026983225</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.989763917212975</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9890683669299062</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9906418203275371</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9877603826458763</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" t="n">
+        <v>21</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9871561711599128</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.9848347327925404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.9905007847468091</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9863879619576181</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9917160574374575</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.9881191416188676</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="n">
+        <v>400</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9854234449234226</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9861011768307386</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.9889985263520042</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.9864200181289061</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.9907442279034873</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9875374788277117</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>21</v>
+      </c>
+      <c r="F8" t="n">
+        <v>500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>18</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9846924928332484</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.985146133179174</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.9889985263520042</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9878342470258968</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.9917160574374575</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.9876774913655563</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>gini</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>150</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9847755178524658</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9814632114151935</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.9827844301601295</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.9867877909273719</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.9862817597689497</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.9844185420248222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>13</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.8268748805871683</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.8086577251796926</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.842807864571653</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.8154401136565022</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.8428246127280945</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.8273210393446222</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9624350795053922</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.9455367976390423</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9682938902993993</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.9624472419109688</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.9650367735341482</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.9607499565777902</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9862806813923686</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.9820324469646149</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.9802179160167925</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9849648832414222</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.9905162072216733</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.9848024269673742</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
+      <c r="F13" t="n">
+        <v>150</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9777663503945369</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.9795182192488896</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.9723756786386794</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.9843260474196867</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.9826680716890173</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.9793308734781618</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>15</v>
+      </c>
+      <c r="F14" t="n">
+        <v>200</v>
+      </c>
+      <c r="G14" t="n">
+        <v>21</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9850344774743822</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.9793058050422392</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.9891717250110007</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.9849878298975374</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.9913037542948692</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.9859607183440058</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>17</v>
+      </c>
+      <c r="F15" t="n">
+        <v>400</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9858502955861703</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.9842008947337588</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.9891511721149359</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.9882685347127076</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.9918370519325963</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.9878615898160337</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9859419079025691</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.9836645759570886</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.9889375881764481</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.9868532508086646</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.993247526687467</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.9877289699064475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>entropy</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>150</v>
+      </c>
+      <c r="G17" t="n">
+        <v>12</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9852143264489701</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.9819171589060189</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.9833446074080839</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9871951616772192</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.9870642026677869</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.9849470914216157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -3125,785 +4753,148 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Conf_id</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Criterion</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>max_depth</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>n_estimators</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>max_features</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>P1</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>P2</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>P3</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
       </c>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>P5</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Promedio</t>
         </is>
       </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
+        <v>0.990122308564267</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9898348447536065</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9881761676421107</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>0.9894727591294215</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>0.9934384728146822</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>0.9902089105808175</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8082813012803404</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.8047662376139391</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.7861722212162833</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.7742819099071137</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.8177520061402811</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.7982507352315914</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>7</v>
-      </c>
-      <c r="F3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.9614932441097477</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.9522535577528214</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.9496338346378987</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.9290591409681976</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.9398414431196858</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.9464562441176703</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" t="n">
-        <v>100</v>
-      </c>
-      <c r="G4" t="n">
-        <v>9</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.985740541262185</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.9827410729132375</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.985667235573898</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.9855146623457041</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.9855509657450032</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.9850428955680055</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F5" t="n">
-        <v>150</v>
-      </c>
-      <c r="G5" t="n">
-        <v>15</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.9852105060606411</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.9841173026983225</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.989763917212975</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.9890683669299062</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.9906418203275371</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.9877603826458763</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" t="n">
-        <v>200</v>
-      </c>
-      <c r="G6" t="n">
-        <v>21</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.9871561711599128</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.9848347327925404</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.9905007847468091</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.9863879619576181</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.9917160574374575</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.9881191416188676</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>17</v>
-      </c>
-      <c r="F7" t="n">
-        <v>400</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.9854234449234226</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.9861011768307386</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.9889985263520042</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.9864200181289061</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.9907442279034873</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.9875374788277117</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>21</v>
-      </c>
-      <c r="F8" t="n">
-        <v>500</v>
-      </c>
-      <c r="G8" t="n">
-        <v>18</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.9846924928332484</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.985146133179174</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.9889985263520042</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.9878342470258968</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.9917160574374575</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.9876774913655563</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>gini</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" t="n">
-        <v>150</v>
-      </c>
-      <c r="G9" t="n">
-        <v>10</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.9847755178524658</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.9814632114151935</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.9827844301601295</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.9867877909273719</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.9862817597689497</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.9844185420248222</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" t="n">
-        <v>13</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.8268748805871683</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.8086577251796926</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.842807864571653</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.8154401136565022</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.8428246127280945</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.8273210393446222</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>7</v>
-      </c>
-      <c r="F11" t="n">
-        <v>30</v>
-      </c>
-      <c r="G11" t="n">
-        <v>15</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.9624350795053922</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.9455367976390423</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.9682938902993993</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.9624472419109688</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.9650367735341482</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.9607499565777902</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>10</v>
-      </c>
-      <c r="F12" t="n">
-        <v>100</v>
-      </c>
-      <c r="G12" t="n">
-        <v>7</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.9862806813923686</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.9820324469646149</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.9802179160167925</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.9849648832414222</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.9905162072216733</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.9848024269673742</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>13</v>
-      </c>
-      <c r="F13" t="n">
-        <v>150</v>
-      </c>
-      <c r="G13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.9777663503945369</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.9795182192488896</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.9723756786386794</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.9843260474196867</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.9826680716890173</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.9793308734781618</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>15</v>
-      </c>
-      <c r="F14" t="n">
-        <v>200</v>
-      </c>
-      <c r="G14" t="n">
-        <v>21</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.9850344774743822</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.9793058050422392</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.9891717250110007</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.9849878298975374</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.9913037542948692</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.9859607183440058</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>17</v>
-      </c>
-      <c r="F15" t="n">
-        <v>400</v>
-      </c>
-      <c r="G15" t="n">
-        <v>11</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.9858502955861703</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.9842008947337588</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.9891511721149359</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.9882685347127076</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.9918370519325963</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.9878615898160337</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>21</v>
-      </c>
-      <c r="F16" t="n">
-        <v>500</v>
-      </c>
-      <c r="G16" t="n">
-        <v>15</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.9859419079025691</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.9836645759570886</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.9889375881764481</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.9868532508086646</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.993247526687467</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.9877289699064475</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>entropy</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>10</v>
-      </c>
-      <c r="F17" t="n">
-        <v>150</v>
-      </c>
-      <c r="G17" t="n">
-        <v>12</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.9852143264489701</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.9819171589060189</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.9833446074080839</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.9871951616772192</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.9870642026677869</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.9849470914216157</v>
+        <v>0.9917</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.990122308564267</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9898348447536065</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9881761676421107</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9894727591294215</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9934384728146822</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9902089105808175</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing for RFC implemented
</commit_message>
<xml_diff>
--- a/Configurations/ConfigurationResults.xlsx
+++ b/Configurations/ConfigurationResults.xlsx
@@ -15,6 +15,7 @@
     <sheet name="CompleteRFC2" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="CompleteRFC3" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="CompleteRFC4" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CompleteRFC5" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1279,6 +1280,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.990122308564267</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9898348447536065</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9881761676421107</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9894727591294215</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9934384728146822</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9902089105808175</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9917</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Part 4 train done
</commit_message>
<xml_diff>
--- a/Configurations/ConfigurationResults.xlsx
+++ b/Configurations/ConfigurationResults.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="11" autoFilterDateGrouping="1" firstSheet="9" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7365" windowWidth="14400" xWindow="38595" yWindow="2775"/>
+    <workbookView activeTab="24" autoFilterDateGrouping="1" firstSheet="22" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7365" windowWidth="14400" xWindow="39270" yWindow="195"/>
   </bookViews>
   <sheets>
     <sheet name="CompleteSVM" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,6 +21,31 @@
     <sheet name="CompleteSVM5" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="CompleteSVM6" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="CompleteRFC6" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CompleteSVM7" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="CompleteNB2" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="CompleteNB3" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="CompleteNB4" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="CompleteNB5" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="CompleteNB6" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="CompleteNB7" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="CompleteNB8" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="CompleteNB9" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="CompleteNB10" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="CompleteNB11" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="CompleteNB12" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CompleteNB13" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="CompleteNB14" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="CompleteNB15" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="CompleteNB16" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="CompleteNB17" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="CompleteNB18" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="CompleteNB19" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="CompleteNB20" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="CompleteNB21" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CompleteNB22" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="CompleteNB23" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="CompleteNB24" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CompleteNB25" sheetId="40" state="visible" r:id="rId40"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -30,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -62,6 +87,16 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -73,12 +108,42 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -152,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -167,6 +232,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1480,7 +1551,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1566,7 +1637,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="5" t="inlineStr">
@@ -1648,7 +1719,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="5" t="inlineStr">
@@ -1730,7 +1801,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="5" t="inlineStr">
@@ -1793,6 +1864,610 @@
       </c>
       <c r="H2" t="n">
         <v>0.9772</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9854031554812726</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.982485649712815</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9842848761628089</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9811654913286757</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9824744744252392</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9831627294221622</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9829</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5425122242821158</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.541545553450009</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5543428811739199</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.5270555720621555</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5410489795757984</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5413010421087996</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.8962505605779085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4298715349686077</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.4270761684768409</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4050427995869613</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.4087789233153506</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.4089993915580249</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.4159537635811571</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.8962505605779085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4298715349686077</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.4270761684768409</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4050427995869613</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.4087789233153506</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.4089993915580249</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.4159537635811571</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.8962505605779085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8962505605779085</v>
       </c>
     </row>
   </sheetData>
@@ -2580,6 +3255,1746 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9193329194737512</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9334685826473618</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9051476119001864</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9183206369233927</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9189986135141607</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9190536728917706</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8962505605779085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9160097769012676</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9285374278759353</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9067317399872582</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.915404578157799</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.920238975963831</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9173844997772183</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8962505605779085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9275330018464631</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9340492406934156</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9130752306328176</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9220795928721632</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.915318293938967</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9224110719967651</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.910039446822825</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8923403265577243</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.898613279560613</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8927600319315524</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8874997180168284</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8962505605779085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9249574697828614</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.934616353829274</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9119387032474127</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9217393973992112</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9169063912633524</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9220316631044223</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9249574697828614</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.934616353829274</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9119387032474127</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9217393973992112</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9169063912633524</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9220316631044223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8878362162945551</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8787072341621498</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8749815110635629</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8877716475182306</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8787086275633624</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8816010473203721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9267516638404367</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9352898348423607</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9139362714606964</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9217919089387989</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9161429825247999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9227825323214185</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9267516638404367</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9352898348423607</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9139362714606964</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9217919089387989</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9161429825247999</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9227825323214185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5485171838816332</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5419006210212522</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5482147010540936</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.5635941667589032</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5275954625744305</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5459644270580626</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8740903917713534</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8797725156777829</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.8773235245793694</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8741286966144658</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8677321740504886</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.874609460538692</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5569730225535083</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.549811077793948</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5610530799938511</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.576207404417198</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5407240717083843</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5569537312933779</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9076759848835793</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9144786105206081</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.8929242438605107</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9020040283120943</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8965631927204679</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.902729212059452</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9076759848835793</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9144786105206081</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.8929242438605107</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9020040283120943</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8965631927204679</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.902729212059452</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -3374,6 +5789,1664 @@
       </c>
       <c r="M17" t="n">
         <v>0.9849470914216157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.933140159671732</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9347369319418086</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9144432340069897</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9343736068775821</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9332487282084385</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9299885321413102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9322665096020011</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9359335331739591</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9177607973280407</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9334309915076849</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9331979437481807</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9305179550719732</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9322665096020011</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9359335331739591</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9177607973280407</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9334309915076849</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9331979437481807</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9305179550719732</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.932751216002933</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9308202831450739</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.932751216002933</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9308202831450739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9318743368869219</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9198473826347945</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9307320312556366</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9320841742778297</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9304446199752036</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9318743368869219</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9198473826347945</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9307320312556366</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9320841742778297</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9304446199752036</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9332135030309648</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9364939069867925</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.917839877878993</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9331537045883479</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9305172137730411</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9332135030309648</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9364939069867925</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.917839877878993</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9331537045883479</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9305172137730411</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.932751216002933</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9308202831450739</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.932751216002933</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9308202831450739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9337895336344664</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9353896148266582</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9165411938442367</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9339230827802154</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9320849853438016</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9303456820858758</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9337895336344664</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9353896148266582</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9165411938442367</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9339230827802154</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9320849853438016</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9303456820858758</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9322880161851809</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9309746200526393</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9305455519160297</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9322880161851809</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9309746200526393</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9305455519160297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7981130985529252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7957795333135528</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7994674256039596</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8206037485173052</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.794554863662476</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8017037339300437</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9318743368869219</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9360281482915955</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.93272708920215</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9300376110458293</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9298748790887222</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9318743368869219</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9360281482915955</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.93272708920215</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9300376110458293</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9298748790887222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.932751216002933</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9308202831450739</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9494</v>
       </c>
     </row>
   </sheetData>
@@ -3483,6 +7556,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.932751216002933</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9376851748208349</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.918707210017115</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9330727385043792</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9318850763801071</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9308202831450739</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9494</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
NB train and test fixed (they were being trained with the labels)
</commit_message>
<xml_diff>
--- a/Configurations/ConfigurationResults.xlsx
+++ b/Configurations/ConfigurationResults.xlsx
@@ -46,6 +46,13 @@
     <sheet name="CompleteNB23" sheetId="38" state="visible" r:id="rId38"/>
     <sheet name="CompleteNB24" sheetId="39" state="visible" r:id="rId39"/>
     <sheet name="CompleteNB25" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="ClinicalNB" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="ClinicalNB1" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="ClinicalNB2" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="LabNB" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="ClinicalNB3" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="LabNB1" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="LabNB2" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -7648,6 +7655,814 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7931283430792027</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7920333509430529</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7955894503171277</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8154063829277552</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.7845617124982224</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.7961438479530721</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9216641870017656</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9200612080359398</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9114584800680022</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9086402948228408</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9205627034707913</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.916477374679868</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9216641870017656</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9200612080359398</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9114584800680022</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9086402948228408</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9205627034707913</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.916477374679868</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9216641870017656</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9200612080359398</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9114584800680022</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9086402948228408</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9205627034707913</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.916477374679868</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9216641870017656</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9200612080359398</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9114584800680022</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9086402948228408</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9205627034707913</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.916477374679868</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Conf_id</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Lab</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gaussian</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5075715144200673</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5049922884524501</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5120882634720421</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.4975575414068923</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.4981614261866363</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5040742067876176</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Lab</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.4119384239633809</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.4275964632551317</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.4409876828343616</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.4248359765209714</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.4195962607612967</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4249909614670285</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lab</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bernoulli</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4119384239633809</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.4275964632551317</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4409876828343616</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.4248359765209714</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.4195962607612967</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.4249909614670285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9216641870017656</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9200612080359398</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9114584800680022</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9086402948228408</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9205627034707913</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.916477374679868</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.4119384239633809</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4275964632551317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4409876828343616</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.4248359765209714</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.4195962607612967</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.4249909614670285</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.6889999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.4119384239633809</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4275964632551317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4409876828343616</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.4248359765209714</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.4195962607612967</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.4249909614670285</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.6889999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>